<commit_message>
My account page test is created
</commit_message>
<xml_diff>
--- a/src/main/java/com/mystore/qa/config/data.xlsx
+++ b/src/main/java/com/mystore/qa/config/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dzmitryrazhkou/Documents/Automation/MyStore/src/main/java/com/mystore/qa/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC47DBD0-EBF3-2448-ABE0-D1981F0CCC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91006F5-26A0-7744-B7CE-4BE6A609F9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19000" activeTab="6" xr2:uid="{16A12737-2736-D94B-B652-76026B2045B5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19000" activeTab="6" xr2:uid="{16A12737-2736-D94B-B652-76026B2045B5}"/>
   </bookViews>
   <sheets>
     <sheet name="sectionWomen" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="getFooterInformation" sheetId="5" r:id="rId4"/>
     <sheet name="getFooterStoreInfo" sheetId="6" r:id="rId5"/>
     <sheet name="createAccount" sheetId="7" r:id="rId6"/>
-    <sheet name="LoginCreateAccountPage" sheetId="8" r:id="rId7"/>
+    <sheet name="LoginCreateAccountPage" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="104">
   <si>
     <t>first</t>
   </si>
@@ -138,12 +138,6 @@
     <t>alexlewis@gmail.com</t>
   </si>
   <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -156,12 +150,6 @@
     <t>years</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>address2</t>
-  </si>
-  <si>
     <t>city</t>
   </si>
   <si>
@@ -330,29 +318,38 @@
     <t>company</t>
   </si>
   <si>
-    <t>Noah Smith LLC</t>
-  </si>
-  <si>
-    <t>Oliver Reyes Corporation</t>
-  </si>
-  <si>
-    <t>EvansLucs LLC</t>
-  </si>
-  <si>
     <t>Taylor Jam</t>
   </si>
   <si>
-    <t>Lewic Corporation</t>
-  </si>
-  <si>
-    <t>noahsmith@gmail.com</t>
+    <t>Lewic LLC</t>
+  </si>
+  <si>
+    <t>Evans LLC</t>
+  </si>
+  <si>
+    <t>Reyes Corporation</t>
+  </si>
+  <si>
+    <t>Smith LLC</t>
+  </si>
+  <si>
+    <t>addressSl</t>
+  </si>
+  <si>
+    <t>addressFl</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>firstName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -387,6 +384,17 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color rgb="FF0066CC"/>
       <name val="Menlo Regular"/>
     </font>
   </fonts>
@@ -429,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -452,26 +460,23 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection hidden="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1093,345 +1098,324 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6597947-744B-674B-94DB-C6CBF85FD531}">
-  <dimension ref="A1:P7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA66764-0456-2846-ABD4-B850DD9718A8}">
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="29.1640625" customWidth="1"/>
-    <col min="9" max="9" width="27.6640625" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" customWidth="1"/>
-    <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="24" customWidth="1"/>
-    <col min="14" max="14" width="27" customWidth="1"/>
-    <col min="15" max="15" width="20.83203125" customWidth="1"/>
+    <col min="1" max="2" width="50.5" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="8" width="36.5" customWidth="1"/>
+    <col min="9" max="9" width="40.83203125" customWidth="1"/>
+    <col min="10" max="10" width="31.33203125" customWidth="1"/>
+    <col min="11" max="11" width="28.33203125" customWidth="1"/>
+    <col min="12" max="12" width="28.1640625" customWidth="1"/>
+    <col min="13" max="14" width="26.83203125" customWidth="1"/>
+    <col min="15" max="15" width="55.6640625" customWidth="1"/>
+    <col min="16" max="16" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:16" ht="21">
+      <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="G1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="M1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="10"/>
+    </row>
+    <row r="2" spans="1:16" ht="18">
+      <c r="A2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="12">
+        <v>13</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="12">
+        <v>1985</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="12">
+        <v>90028</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" s="10"/>
+    </row>
+    <row r="3" spans="1:16" ht="18">
+      <c r="A3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="12">
+        <v>29</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="12">
+        <v>1974</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" s="10"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="14">
-        <v>13</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="14">
-        <v>1985</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M2" s="14">
-        <v>90028</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2" s="10"/>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="I3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="J3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="K3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="14">
-        <v>29</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="L3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="14">
-        <v>1974</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="I3" s="8" t="s">
+      <c r="M3" s="12">
+        <v>19121</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="O3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="P3" s="10"/>
+    </row>
+    <row r="4" spans="1:16" ht="18">
+      <c r="A4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="C4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M3" s="14">
-        <v>19121</v>
-      </c>
-      <c r="N3" s="8" t="s">
+      <c r="D4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="E4" s="12">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="P3" s="10"/>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="G4" s="12">
+        <v>1999</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="J4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="K4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="14">
-        <v>3</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="L4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="14">
-        <v>1999</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="I4" s="8" t="s">
+      <c r="M4" s="12">
+        <v>60007</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="O4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" spans="1:16" ht="18">
+      <c r="A5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="C5" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M4" s="14">
-        <v>60007</v>
-      </c>
-      <c r="N4" s="8" t="s">
+      <c r="D5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="E5" s="12">
+        <v>5</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="P4" s="10"/>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="G5" s="12">
+        <v>1989</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="J5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="K5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="14">
-        <v>5</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="L5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="14">
-        <v>1989</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="I5" s="8" t="s">
+      <c r="M5" s="12">
+        <v>33101</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="O5" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="1:16" ht="18">
+      <c r="A6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="C6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="M5" s="14">
-        <v>33101</v>
-      </c>
-      <c r="N5" s="8" t="s">
+      <c r="D6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="E6" s="12">
+        <v>19</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="P5" s="10"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="G6" s="12">
+        <v>1993</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="J6" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="K6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="14">
-        <v>19</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="L6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G6" s="14">
-        <v>1993</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" s="8" t="s">
+      <c r="M6" s="12">
+        <v>75001</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="O6" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="M6" s="14">
-        <v>75001</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="P6" s="10"/>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{1F3455F4-4478-7340-8882-D48EECBE067A}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{37E1AC52-589A-2B45-824E-B818D7CC8CEB}"/>
-    <hyperlink ref="A6" r:id="rId3" xr:uid="{E814DE6A-3554-7041-B2B9-D43DEB0EBB3E}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{87E9A337-CE18-E048-994D-5A939F2E128A}"/>
-    <hyperlink ref="A4" r:id="rId5" xr:uid="{090140FD-6583-9C47-B9EF-C1C7F8DA5AAD}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1151CEBB-EBEF-5D44-B606-957FA8259852}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{7A51B345-05B7-9C4D-A4BE-7E8F7A26180B}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{E9E0066F-79FC-EA49-B50C-244BAAA3F289}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>